<commit_message>
Remove some warnings on GreenPAK configuration (ex. Unused cell has non-default LUT setting)
</commit_message>
<xml_diff>
--- a/doc/KeplerX-bus-access-cycle.xlsx
+++ b/doc/KeplerX-bus-access-cycle.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10116"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ohnaka/work/X68000/X68k-KeplerX-RTL/doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD66D604-244A-F249-AD96-B5D08FF500D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB9E3E7D-97B7-CD46-BF8B-BD35B4F1DE12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13200" yWindow="500" windowWidth="40040" windowHeight="32980" xr2:uid="{0684F262-CA78-2C4E-8CA0-6BF7C1AAA7E6}"/>
+    <workbookView xWindow="20680" yWindow="1880" windowWidth="40040" windowHeight="28740" xr2:uid="{0684F262-CA78-2C4E-8CA0-6BF7C1AAA7E6}"/>
   </bookViews>
   <sheets>
     <sheet name="GreenPak BusMode New" sheetId="7" r:id="rId1"/>
@@ -993,8 +993,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05004F82-66C8-9E4F-B444-38C10502323D}">
   <dimension ref="B2:V78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="81" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="F67" sqref="F67"/>
+    <sheetView tabSelected="1" zoomScale="81" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="R11" sqref="R11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="20"/>

</xml_diff>

<commit_message>
Optimize GreenPAK logic (Bus-master cycle shoud be changed)
</commit_message>
<xml_diff>
--- a/doc/KeplerX-bus-access-cycle.xlsx
+++ b/doc/KeplerX-bus-access-cycle.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ohnaka/work/X68000/X68k-KeplerX-RTL/doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB9E3E7D-97B7-CD46-BF8B-BD35B4F1DE12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43E37B56-004A-4B42-99BF-B399F43034A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20680" yWindow="1880" windowWidth="40040" windowHeight="28740" xr2:uid="{0684F262-CA78-2C4E-8CA0-6BF7C1AAA7E6}"/>
+    <workbookView xWindow="17820" yWindow="1920" windowWidth="40040" windowHeight="28740" xr2:uid="{0684F262-CA78-2C4E-8CA0-6BF7C1AAA7E6}"/>
   </bookViews>
   <sheets>
     <sheet name="GreenPak BusMode New" sheetId="7" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="355" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="356" uniqueCount="92">
   <si>
     <t>MODE</t>
     <phoneticPr fontId="1"/>
@@ -991,10 +991,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05004F82-66C8-9E4F-B444-38C10502323D}">
-  <dimension ref="B2:V78"/>
+  <dimension ref="B2:V79"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="81" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="R11" sqref="R11"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="20"/>
@@ -1606,20 +1606,42 @@
         <f t="shared" si="0"/>
         <v>1100</v>
       </c>
-      <c r="E17" s="7"/>
-      <c r="F17" s="2"/>
-      <c r="G17" s="7"/>
-      <c r="H17" s="7"/>
+      <c r="E17" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="F17" s="2">
+        <v>0</v>
+      </c>
+      <c r="G17" s="7">
+        <v>1</v>
+      </c>
+      <c r="H17" s="7">
+        <v>1</v>
+      </c>
       <c r="I17" s="7"/>
-      <c r="J17" s="7"/>
-      <c r="K17" s="7"/>
-      <c r="L17" s="7"/>
+      <c r="J17" s="7">
+        <v>0</v>
+      </c>
+      <c r="K17" s="7">
+        <v>0</v>
+      </c>
+      <c r="L17" s="7">
+        <v>0</v>
+      </c>
       <c r="M17" s="7"/>
-      <c r="N17" s="7"/>
-      <c r="O17" s="7"/>
+      <c r="N17" s="7">
+        <v>0</v>
+      </c>
+      <c r="O17" s="7">
+        <v>1</v>
+      </c>
       <c r="P17" s="7"/>
-      <c r="Q17" s="7"/>
-      <c r="R17" s="7"/>
+      <c r="Q17" s="7">
+        <v>1</v>
+      </c>
+      <c r="R17" s="7">
+        <v>0</v>
+      </c>
     </row>
     <row r="18" spans="3:22">
       <c r="C18">
@@ -1630,7 +1652,7 @@
         <v>1101</v>
       </c>
       <c r="E18" s="7" t="s">
-        <v>15</v>
+        <v>68</v>
       </c>
       <c r="F18" s="2">
         <v>0</v>
@@ -1660,10 +1682,10 @@
       </c>
       <c r="P18" s="7"/>
       <c r="Q18" s="7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R18" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19" spans="3:22">
@@ -3788,7 +3810,7 @@
         <v>34</v>
       </c>
       <c r="F67" s="9">
-        <f t="shared" ref="F67:H78" si="16">VLOOKUP($D67,$D$5:$R$20,F$23)</f>
+        <f t="shared" ref="F67:H79" si="16">VLOOKUP($D67,$D$5:$R$20,F$23)</f>
         <v>1</v>
       </c>
       <c r="G67">
@@ -3800,7 +3822,7 @@
         <v>1</v>
       </c>
       <c r="J67">
-        <f t="shared" ref="J67:L78" si="17">VLOOKUP($D67,$D$5:$R$20,J$23)</f>
+        <f t="shared" ref="J67:L79" si="17">VLOOKUP($D67,$D$5:$R$20,J$23)</f>
         <v>0</v>
       </c>
       <c r="K67">
@@ -3812,7 +3834,7 @@
         <v>1</v>
       </c>
       <c r="N67">
-        <f t="shared" ref="N67:O78" si="18">VLOOKUP($D67,$D$5:$R$20,N$23)</f>
+        <f t="shared" ref="N67:O79" si="18">VLOOKUP($D67,$D$5:$R$20,N$23)</f>
         <v>0</v>
       </c>
       <c r="O67">
@@ -3820,7 +3842,7 @@
         <v>1</v>
       </c>
       <c r="Q67">
-        <f t="shared" ref="Q67:R78" si="19">VLOOKUP($D67,$D$5:$R$20,Q$23)</f>
+        <f t="shared" ref="Q67:R79" si="19">VLOOKUP($D67,$D$5:$R$20,Q$23)</f>
         <v>0</v>
       </c>
       <c r="R67">
@@ -3900,7 +3922,7 @@
         <v>9</v>
       </c>
       <c r="D69" s="3" t="str">
-        <f t="shared" ref="D69:D77" si="20">DEC2BIN(C69,4)</f>
+        <f t="shared" ref="D69:D78" si="20">DEC2BIN(C69,4)</f>
         <v>1001</v>
       </c>
       <c r="E69" s="3" t="s">
@@ -4147,9 +4169,7 @@
         <f t="shared" si="20"/>
         <v>1101</v>
       </c>
-      <c r="E73" s="3" t="s">
-        <v>36</v>
-      </c>
+      <c r="E73" s="3"/>
       <c r="F73" s="2">
         <f t="shared" si="16"/>
         <v>0</v>
@@ -4182,34 +4202,31 @@
         <f t="shared" si="18"/>
         <v>1</v>
       </c>
-      <c r="Q73" s="5">
+      <c r="Q73">
         <f t="shared" si="19"/>
-        <v>1</v>
-      </c>
-      <c r="R73" s="1">
+        <v>0</v>
+      </c>
+      <c r="R73">
         <f t="shared" si="19"/>
-        <v>0</v>
-      </c>
-      <c r="T73" s="8">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="T73">
+        <v>1</v>
       </c>
       <c r="U73" s="8">
         <v>0</v>
-      </c>
-      <c r="V73" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="74" spans="3:22">
       <c r="C74">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D74" s="3" t="str">
         <f t="shared" si="20"/>
-        <v>1101</v>
+        <v>1100</v>
       </c>
       <c r="E74" s="3" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="F74" s="2">
         <f t="shared" si="16"/>
@@ -4243,7 +4260,7 @@
         <f t="shared" si="18"/>
         <v>1</v>
       </c>
-      <c r="Q74">
+      <c r="Q74" s="5">
         <f t="shared" si="19"/>
         <v>1</v>
       </c>
@@ -4258,16 +4275,16 @@
         <v>0</v>
       </c>
       <c r="V74" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="75" spans="3:22">
       <c r="C75">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D75" s="3" t="str">
         <f t="shared" si="20"/>
-        <v>1101</v>
+        <v>1100</v>
       </c>
       <c r="E75" s="3" t="s">
         <v>47</v>
@@ -4319,19 +4336,19 @@
         <v>0</v>
       </c>
       <c r="V75" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="76" spans="3:22">
       <c r="C76">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D76" s="3" t="str">
         <f t="shared" si="20"/>
-        <v>1101</v>
+        <v>1100</v>
       </c>
       <c r="E76" s="3" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="F76" s="2">
         <f t="shared" si="16"/>
@@ -4380,19 +4397,19 @@
         <v>0</v>
       </c>
       <c r="V76" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
     </row>
     <row r="77" spans="3:22">
       <c r="C77">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="D77" s="3" t="str">
         <f t="shared" si="20"/>
-        <v>1001</v>
+        <v>1100</v>
       </c>
       <c r="E77" s="3" t="s">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="F77" s="2">
         <f t="shared" si="16"/>
@@ -4414,9 +4431,9 @@
         <f t="shared" si="17"/>
         <v>0</v>
       </c>
-      <c r="L77">
+      <c r="L77" s="1">
         <f t="shared" si="17"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N77">
         <f t="shared" si="18"/>
@@ -4428,40 +4445,40 @@
       </c>
       <c r="Q77">
         <f t="shared" si="19"/>
-        <v>0</v>
-      </c>
-      <c r="R77">
+        <v>1</v>
+      </c>
+      <c r="R77" s="1">
         <f t="shared" si="19"/>
-        <v>1</v>
-      </c>
-      <c r="T77">
-        <v>1</v>
-      </c>
-      <c r="U77">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="T77" s="8">
+        <v>0</v>
+      </c>
+      <c r="U77" s="8">
+        <v>0</v>
       </c>
       <c r="V77" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="78" spans="3:22">
       <c r="C78">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D78" s="3" t="str">
-        <f>DEC2BIN(C78,4)</f>
-        <v>1000</v>
+        <f t="shared" si="20"/>
+        <v>1001</v>
       </c>
       <c r="E78" s="3" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="F78" s="2">
         <f t="shared" si="16"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G78">
         <f t="shared" si="16"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H78">
         <f t="shared" si="16"/>
@@ -4499,6 +4516,67 @@
         <v>1</v>
       </c>
       <c r="U78">
+        <v>1</v>
+      </c>
+      <c r="V78" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="79" spans="3:22">
+      <c r="C79">
+        <v>8</v>
+      </c>
+      <c r="D79" s="3" t="str">
+        <f>DEC2BIN(C79,4)</f>
+        <v>1000</v>
+      </c>
+      <c r="E79" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="F79" s="2">
+        <f t="shared" si="16"/>
+        <v>1</v>
+      </c>
+      <c r="G79">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+      <c r="H79">
+        <f t="shared" si="16"/>
+        <v>1</v>
+      </c>
+      <c r="J79">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="K79">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="L79">
+        <f t="shared" si="17"/>
+        <v>1</v>
+      </c>
+      <c r="N79">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="O79">
+        <f t="shared" si="18"/>
+        <v>1</v>
+      </c>
+      <c r="Q79">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="R79">
+        <f t="shared" si="19"/>
+        <v>1</v>
+      </c>
+      <c r="T79">
+        <v>1</v>
+      </c>
+      <c r="U79">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update bus master cycle.
</commit_message>
<xml_diff>
--- a/doc/KeplerX-bus-access-cycle.xlsx
+++ b/doc/KeplerX-bus-access-cycle.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ohnaka/work/X68000/X68k-KeplerX-RTL/doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43E37B56-004A-4B42-99BF-B399F43034A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1168D70-2396-1E47-B161-E87C851831DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17820" yWindow="1920" windowWidth="40040" windowHeight="28740" xr2:uid="{0684F262-CA78-2C4E-8CA0-6BF7C1AAA7E6}"/>
+    <workbookView xWindow="31720" yWindow="1920" windowWidth="33680" windowHeight="23220" xr2:uid="{0684F262-CA78-2C4E-8CA0-6BF7C1AAA7E6}"/>
   </bookViews>
   <sheets>
     <sheet name="GreenPak BusMode New" sheetId="7" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="356" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="357" uniqueCount="92">
   <si>
     <t>MODE</t>
     <phoneticPr fontId="1"/>
@@ -993,8 +993,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05004F82-66C8-9E4F-B444-38C10502323D}">
   <dimension ref="B2:V79"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="81" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView tabSelected="1" topLeftCell="B33" zoomScale="88" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="E77" sqref="E77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="20"/>
@@ -3215,7 +3215,7 @@
         <v>1011</v>
       </c>
       <c r="E55" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F55" s="2">
         <f t="shared" si="11"/>
@@ -3269,11 +3269,11 @@
     </row>
     <row r="56" spans="3:22">
       <c r="C56">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="D56" s="3" t="str">
         <f t="shared" si="15"/>
-        <v>1011</v>
+        <v>1111</v>
       </c>
       <c r="E56" s="3" t="s">
         <v>30</v>
@@ -3292,11 +3292,11 @@
       </c>
       <c r="J56">
         <f t="shared" si="12"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K56">
         <f t="shared" si="12"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L56" s="1">
         <f t="shared" si="12"/>
@@ -3337,7 +3337,7 @@
         <v>1111</v>
       </c>
       <c r="E57" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F57" s="2">
         <f t="shared" si="11"/>
@@ -3581,7 +3581,7 @@
         <v>1010</v>
       </c>
       <c r="E61" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F61" s="2">
         <f t="shared" si="11"/>
@@ -3987,7 +3987,7 @@
         <v>1011</v>
       </c>
       <c r="E70" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F70" s="2">
         <f t="shared" si="16"/>
@@ -4041,11 +4041,11 @@
     </row>
     <row r="71" spans="3:22">
       <c r="C71">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="D71" s="3" t="str">
         <f t="shared" si="20"/>
-        <v>1011</v>
+        <v>1111</v>
       </c>
       <c r="E71" s="3" t="s">
         <v>30</v>
@@ -4064,11 +4064,11 @@
       </c>
       <c r="J71">
         <f t="shared" si="17"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K71">
         <f t="shared" si="17"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L71" s="1">
         <f t="shared" si="17"/>
@@ -4109,7 +4109,7 @@
         <v>1111</v>
       </c>
       <c r="E72" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F72" s="2">
         <f t="shared" si="16"/>
@@ -4169,7 +4169,9 @@
         <f t="shared" si="20"/>
         <v>1101</v>
       </c>
-      <c r="E73" s="3"/>
+      <c r="E73" s="3" t="s">
+        <v>36</v>
+      </c>
       <c r="F73" s="2">
         <f t="shared" si="16"/>
         <v>0</v>
@@ -4463,22 +4465,22 @@
     </row>
     <row r="78" spans="3:22">
       <c r="C78">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D78" s="3" t="str">
         <f t="shared" si="20"/>
-        <v>1001</v>
+        <v>1000</v>
       </c>
       <c r="E78" s="3" t="s">
         <v>40</v>
       </c>
       <c r="F78" s="2">
         <f t="shared" si="16"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G78">
         <f t="shared" si="16"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H78">
         <f t="shared" si="16"/>
@@ -4524,18 +4526,18 @@
     </row>
     <row r="79" spans="3:22">
       <c r="C79">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="D79" s="3" t="str">
         <f>DEC2BIN(C79,4)</f>
-        <v>1000</v>
+        <v>0000</v>
       </c>
       <c r="E79" s="3" t="s">
         <v>34</v>
       </c>
       <c r="F79" s="2">
         <f t="shared" si="16"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G79">
         <f t="shared" si="16"/>
@@ -4592,7 +4594,7 @@
   <dimension ref="B2:V76"/>
   <sheetViews>
     <sheetView topLeftCell="B2" zoomScale="81" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17:R17"/>
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="20"/>

</xml_diff>